<commit_message>
modified:   Efemerides_transm/Ej_1-e_RSW_ant.py 	modified:   Efemerides_transm/Ej_1-e_V2.py 	modified:   Efemerides_transm/TP_1_c.xlsx 	modified:   Efemerides_transm/para_enviar/Ej_1-e_V2.py 	new file:   Practica_2/ifag0780.01n
</commit_message>
<xml_diff>
--- a/Efemerides_transm/TP_1_c.xlsx
+++ b/Efemerides_transm/TP_1_c.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/971884e4c0dcab22/Documentos/Curso_Pos_Satelit/Efemerides_transm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1437" documentId="8_{41CBE948-4A59-426F-B6A1-786314178200}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3173020C-CC65-46B4-9253-F5DC34EA6716}"/>
+  <xr:revisionPtr revIDLastSave="1503" documentId="8_{41CBE948-4A59-426F-B6A1-786314178200}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{67DF8071-F791-4290-9313-1686C737F87E}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{C4CFFAFD-BFD9-4F39-9C3C-01FBA7C8A499}"/>
+    <workbookView xWindow="7560" yWindow="570" windowWidth="12930" windowHeight="10230" activeTab="2" xr2:uid="{C4CFFAFD-BFD9-4F39-9C3C-01FBA7C8A499}"/>
   </bookViews>
   <sheets>
     <sheet name="transmitidas" sheetId="1" r:id="rId1"/>
@@ -1451,7 +1451,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="22">
+  <numFmts count="25">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
@@ -1473,7 +1473,10 @@
     <numFmt numFmtId="181" formatCode="_ * #,##0.0000000000000000_ ;_ * \-#,##0.0000000000000000_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="182" formatCode="0.00000000000E+00"/>
     <numFmt numFmtId="183" formatCode="0.0000000"/>
-    <numFmt numFmtId="185" formatCode="0.0000000000000"/>
+    <numFmt numFmtId="184" formatCode="0.0000000000000"/>
+    <numFmt numFmtId="188" formatCode="0.00000000000000000"/>
+    <numFmt numFmtId="190" formatCode="0.0000000000000000000"/>
+    <numFmt numFmtId="191" formatCode="_ * #,##0.000_ ;_ * \-#,##0.000_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -1570,7 +1573,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1619,12 +1622,15 @@
     <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="184" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="183" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="185" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="183" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="188" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="190" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="191" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -3313,7 +3319,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0CAA84F-85F7-4054-BEB1-66776AF2C5EB}">
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
@@ -4089,11 +4095,11 @@
       <c r="A6" t="s">
         <v>51</v>
       </c>
-      <c r="B6" s="40">
+      <c r="B6" s="43">
         <f>DATE(A5,B5,C5)+TIME(D5,E5,F5)</f>
         <v>36969.010416666664</v>
       </c>
-      <c r="C6" s="40"/>
+      <c r="C6" s="43"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -4687,8 +4693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BB902F2-1DD0-42F5-AAF6-FD2395C5A396}">
   <dimension ref="A1:R59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4707,7 +4713,7 @@
     <col min="15" max="15" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>121</v>
       </c>
@@ -4716,7 +4722,7 @@
         <v>1106</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>52</v>
       </c>
@@ -4725,16 +4731,19 @@
         <v>29226</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>58</v>
       </c>
       <c r="B3" s="30">
-        <v>398600500000000</v>
+        <v>398600441800000</v>
       </c>
       <c r="C3" s="9"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>398600441800000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>57</v>
       </c>
@@ -4743,11 +4752,11 @@
       </c>
       <c r="C4" s="9"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="C5" s="9"/>
     </row>
-    <row r="6" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="D6" s="3" t="s">
         <v>66</v>
       </c>
@@ -4764,7 +4773,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>60</v>
       </c>
@@ -4786,7 +4795,7 @@
         <v>87299.999999790452</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>126</v>
       </c>
@@ -4794,9 +4803,9 @@
         <f>transmitidas!B23</f>
         <v>79200</v>
       </c>
-      <c r="D8" s="43"/>
-    </row>
-    <row r="9" spans="1:9" ht="21.75" x14ac:dyDescent="0.4">
+      <c r="D8" s="42"/>
+    </row>
+    <row r="9" spans="1:10" ht="21.75" x14ac:dyDescent="0.4">
       <c r="A9" s="22" t="s">
         <v>61</v>
       </c>
@@ -4821,8 +4830,9 @@
         <f>F9*$B$4</f>
         <v>0.59066132688270001</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" ht="21.75" x14ac:dyDescent="0.4">
+      <c r="J9" s="28"/>
+    </row>
+    <row r="10" spans="1:10" ht="21.75" x14ac:dyDescent="0.4">
       <c r="A10" s="22" t="s">
         <v>100</v>
       </c>
@@ -4848,7 +4858,7 @@
         <v>-0.45940325424209999</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="22"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
@@ -4856,7 +4866,7 @@
       <c r="E11" s="27"/>
       <c r="F11" s="27"/>
     </row>
-    <row r="12" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="22"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -4864,11 +4874,11 @@
       <c r="E12" s="27"/>
       <c r="F12" s="27"/>
     </row>
-    <row r="13" spans="1:9" ht="19.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" ht="19.5" x14ac:dyDescent="0.35">
       <c r="A13" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="B13" s="29">
+      <c r="B13" s="19">
         <f>transmitidas!E21</f>
         <v>-2.93479942981</v>
       </c>
@@ -4881,7 +4891,7 @@
         <v>-0.83438569421099995</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>96</v>
       </c>
@@ -4898,7 +4908,7 @@
         <v>5.2283601835399996E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -4915,7 +4925,7 @@
         <v>5153.59644699</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>63</v>
       </c>
@@ -4953,9 +4963,9 @@
       <c r="A18" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B18" s="23">
+      <c r="B18" s="40">
         <f>B13+(SQRT($B$3/B16/B16/B16)+B17)*($E$7-$E$9)</f>
-        <v>-1.7532942457867327</v>
+        <v>-1.7532943320404997</v>
       </c>
       <c r="C18" s="23"/>
       <c r="D18" s="4" t="s">
@@ -4963,7 +4973,7 @@
       </c>
       <c r="E18" s="34">
         <f>E13+(SQRT($B$3/E16/E16/E16)+E17)*(E7-E10)</f>
-        <v>-1.7533351066769214</v>
+        <v>-1.7533350395906879</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
@@ -5021,9 +5031,9 @@
       <c r="A22" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B22" s="23">
+      <c r="B22" s="35">
         <f>Iterate!B24</f>
-        <v>-1.7584320390771977</v>
+        <v>-1.7584321252469055</v>
       </c>
       <c r="C22" s="23"/>
       <c r="D22" s="4" t="s">
@@ -5031,7 +5041,7 @@
       </c>
       <c r="E22" s="34">
         <f>Iterate!C24</f>
-        <v>-1.7584716600726431</v>
+        <v>-1.7584715930517871</v>
       </c>
       <c r="J22" s="3">
         <f>COS(-B21)</f>
@@ -5062,15 +5072,15 @@
       </c>
       <c r="B23" s="26">
         <f>B16*(1-B14*COS(B22))</f>
-        <v>26585457.605943941</v>
+        <v>26585457.617702439</v>
       </c>
       <c r="C23" s="26"/>
       <c r="D23" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="E23" s="42">
+      <c r="E23" s="41">
         <f>E16*(1-E14*COS(E22))</f>
-        <v>26585464.765958052</v>
+        <v>26585464.756814755</v>
       </c>
       <c r="I23" t="s">
         <v>118</v>
@@ -5105,17 +5115,17 @@
       <c r="A24" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B24" s="35">
+      <c r="B24" s="34">
         <f>2*ATAN(TAN(B22/2)*SQRT(1+B14)/SQRT(1-B14))</f>
-        <v>-1.7635673514167107</v>
+        <v>-1.7635674375012638</v>
       </c>
       <c r="C24" s="23"/>
       <c r="D24" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="E24" s="41">
+      <c r="E24" s="40">
         <f>2*ATAN(TAN(E22/2)*SQRT(1+E14)/SQRT(1-E14))</f>
-        <v>-1.7636057331682027</v>
+        <v>-1.763605666213576</v>
       </c>
       <c r="J24" s="3">
         <v>0</v>
@@ -5159,15 +5169,15 @@
       </c>
       <c r="B26" s="35">
         <f>B25+B24</f>
-        <v>-3.4722838730567105</v>
+        <v>-3.4722839591412638</v>
       </c>
       <c r="C26" s="23"/>
       <c r="D26" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="E26" s="41">
+      <c r="E26" s="40">
         <f>E25+E24</f>
-        <v>-3.4722832417082028</v>
+        <v>-3.4722831747535761</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
@@ -5210,7 +5220,7 @@
       </c>
       <c r="B29" s="23">
         <f>B25+B27*COS(2*B26)+B28*SIN(2*B26)</f>
-        <v>-1.7087243216554786</v>
+        <v>-1.708724321655976</v>
       </c>
       <c r="C29" s="23"/>
       <c r="D29" s="4" t="s">
@@ -5218,7 +5228,7 @@
       </c>
       <c r="E29" s="23">
         <f>E25+E27*COS(2*E26)+E28*SIN(2*E26)</f>
-        <v>-1.7086859436174786</v>
+        <v>-1.7086859436170656</v>
       </c>
       <c r="J29" s="3">
         <f>COS(B39)</f>
@@ -5327,9 +5337,9 @@
       <c r="A32" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="B32" s="26">
+      <c r="B32" s="46">
         <f>B23+B30*COS(2*B26)+B31*SIN(2*B26)</f>
-        <v>26585702.041017018</v>
+        <v>26585702.052761093</v>
       </c>
       <c r="C32" s="26"/>
       <c r="D32" s="4" t="s">
@@ -5337,7 +5347,7 @@
       </c>
       <c r="E32" s="26">
         <f>E23+E30*COS(2*E26)+E31*SIN(2*E26)</f>
-        <v>26585702.384047892</v>
+        <v>26585702.374913916</v>
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
@@ -5432,7 +5442,7 @@
       </c>
       <c r="B37" s="38">
         <f>B33+B34*COS(2*B26)+B35*SIN(2*B26)+B36*($E$7-$E$9)</f>
-        <v>0.96342013675111937</v>
+        <v>0.96342013675111871</v>
       </c>
       <c r="C37" s="28"/>
       <c r="D37" s="4" t="s">
@@ -5440,7 +5450,7 @@
       </c>
       <c r="E37" s="28">
         <f>E33+E34*COS(2*E26)+E35*SIN(2*E26)+E36*($E$7-$E$10)</f>
-        <v>0.96341840162262393</v>
+        <v>0.96341840162261672</v>
       </c>
       <c r="I37" t="s">
         <v>85</v>
@@ -5450,11 +5460,11 @@
       </c>
       <c r="K37" s="3">
         <f>COS(-B37)</f>
-        <v>0.57071489002111575</v>
+        <v>0.57071489002111631</v>
       </c>
       <c r="L37" s="3">
         <f>SIN(-B37)</f>
-        <v>-0.82114829008418799</v>
+        <v>-0.82114829008418755</v>
       </c>
       <c r="O37" t="s">
         <v>85</v>
@@ -5464,11 +5474,11 @@
       </c>
       <c r="Q37" s="3">
         <f>COS(-E37)</f>
-        <v>0.57071631481805374</v>
+        <v>0.57071631481805973</v>
       </c>
       <c r="R37" s="3">
         <f>SIN(-E37)</f>
-        <v>-0.82114729981928336</v>
+        <v>-0.82114729981927925</v>
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
@@ -5477,22 +5487,22 @@
       </c>
       <c r="K38" s="3">
         <f>-SIN(-B37)</f>
-        <v>0.82114829008418799</v>
+        <v>0.82114829008418755</v>
       </c>
       <c r="L38" s="3">
         <f>COS(-B37)</f>
-        <v>0.57071489002111575</v>
+        <v>0.57071489002111631</v>
       </c>
       <c r="P38" s="3">
         <v>0</v>
       </c>
       <c r="Q38" s="3">
         <f>-SIN(-E37)</f>
-        <v>0.82114729981928336</v>
+        <v>0.82114729981927925</v>
       </c>
       <c r="R38" s="3">
         <f>COS(-E37)</f>
-        <v>0.57071631481805374</v>
+        <v>0.57071631481805973</v>
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
@@ -5518,14 +5528,14 @@
       </c>
       <c r="B40" s="34">
         <f>B29+B24</f>
-        <v>-3.4722916730721893</v>
+        <v>-3.4722917591572395</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>105</v>
       </c>
       <c r="E40" s="23">
         <f>E29+E24</f>
-        <v>-3.4722916767856811</v>
+        <v>-3.4722916098306413</v>
       </c>
     </row>
     <row r="42" spans="1:18" ht="18" x14ac:dyDescent="0.35">
@@ -5534,13 +5544,13 @@
       </c>
       <c r="B42" s="36">
         <f>B32*COS(B40)</f>
-        <v>-25145171.72801993</v>
+        <v>-25145170.995999191</v>
       </c>
       <c r="C42" s="28"/>
       <c r="D42" s="28"/>
       <c r="E42" s="28">
         <f>E32*COS(E40)</f>
-        <v>-25145172.0204072</v>
+        <v>-25145172.589756846</v>
       </c>
     </row>
     <row r="43" spans="1:18" ht="18" x14ac:dyDescent="0.35">
@@ -5549,12 +5559,12 @@
       </c>
       <c r="B43" s="36">
         <f>B32*SIN(B40)</f>
-        <v>8632490.4739086479</v>
+        <v>8632492.6423453391</v>
       </c>
       <c r="C43" s="28"/>
       <c r="E43" s="28">
         <f>E32*SIN(E40)</f>
-        <v>8632490.6786686201</v>
+        <v>8632488.9921067692</v>
       </c>
       <c r="J43" s="3">
         <f>J29*J22+K29*J23+L29*J24</f>
@@ -5666,15 +5676,15 @@
       </c>
       <c r="B48" s="28">
         <f>J50*B42+K50*B43+L50*B44</f>
-        <v>581887.39881280623</v>
+        <v>581888.74276992586</v>
       </c>
       <c r="D48" s="33">
         <f>E48-B48</f>
-        <v>-6.1110436879098415</v>
+        <v>-8.5003034053370357</v>
       </c>
       <c r="E48" s="28">
         <f>P50*E42+Q50*E43+R50*E44</f>
-        <v>581881.28776911832</v>
+        <v>581880.24246652052</v>
       </c>
       <c r="G48" s="26">
         <f>precisas!C7*1000</f>
@@ -5687,15 +5697,15 @@
       </c>
       <c r="B49" s="28">
         <f>J51*B42+K51*B43+L51*B44</f>
-        <v>25616661.59030547</v>
+        <v>25616661.079241697</v>
       </c>
       <c r="D49" s="33">
         <f t="shared" ref="D49:D50" si="0">E49-B49</f>
-        <v>2.8137903437018394</v>
+        <v>3.7223471961915493</v>
       </c>
       <c r="E49" s="28">
         <f>P51*E42+Q51*E43+R51*E44</f>
-        <v>25616664.404095814</v>
+        <v>25616664.801588893</v>
       </c>
       <c r="G49" s="26">
         <f>precisas!D7*1000</f>
@@ -5708,15 +5718,15 @@
       </c>
       <c r="B50" s="28">
         <f>J52*B42+K52*B43+L52*B44</f>
-        <v>7088554.791818128</v>
+        <v>7088556.5724262055</v>
       </c>
       <c r="D50" s="33">
         <f t="shared" si="0"/>
-        <v>-8.3803142579272389</v>
+        <v>-11.545838080346584</v>
       </c>
       <c r="E50" s="28">
         <f>P52*E42+Q52*E43+R52*E44</f>
-        <v>7088546.41150387</v>
+        <v>7088545.0265881252</v>
       </c>
       <c r="G50" s="26">
         <f>precisas!E7*1000</f>
@@ -5728,11 +5738,11 @@
       </c>
       <c r="K50" s="3">
         <f>J43*K36+K43*K37+L43*K38</f>
-        <v>0.56241361433773052</v>
+        <v>0.56241361433773107</v>
       </c>
       <c r="L50" s="3">
         <f>J43*L36+K43*L37+L43*L38</f>
-        <v>-0.80920436072100443</v>
+        <v>-0.80920436072100399</v>
       </c>
       <c r="P50" s="3">
         <f>P43*P36+Q43*P37+R43*P38</f>
@@ -5740,11 +5750,11 @@
       </c>
       <c r="Q50" s="3">
         <f>P43*Q36+Q43*Q37+R43*Q38</f>
-        <v>0.56241494913565837</v>
+        <v>0.56241494913566437</v>
       </c>
       <c r="R50" s="3">
         <f>P43*R36+Q43*R37+R43*R38</f>
-        <v>-0.80920328518727735</v>
+        <v>-0.80920328518727336</v>
       </c>
     </row>
     <row r="51" spans="1:18" ht="18" x14ac:dyDescent="0.35">
@@ -5757,11 +5767,11 @@
       </c>
       <c r="K51" s="3">
         <f>J44*K36+K44*K37+L44*K38</f>
-        <v>9.6986659388726304E-2</v>
+        <v>9.6986659388726401E-2</v>
       </c>
       <c r="L51" s="3">
         <f>J44*L36+K44*L37+L44*L38</f>
-        <v>-0.13954503537674226</v>
+        <v>-0.13954503537674218</v>
       </c>
       <c r="O51" s="4" t="s">
         <v>125</v>
@@ -5772,11 +5782,11 @@
       </c>
       <c r="Q51" s="3">
         <f>P44*Q36+Q44*Q37+R44*Q38</f>
-        <v>9.6987303232096186E-2</v>
+        <v>9.69873032320972E-2</v>
       </c>
       <c r="R51" s="3">
         <f>P44*R36+Q44*R37+R44*R38</f>
-        <v>-0.13954544508015265</v>
+        <v>-0.13954544508015196</v>
       </c>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.25">
@@ -5786,11 +5796,11 @@
       </c>
       <c r="K52" s="3">
         <f>J45*K36+K45*K37+L45*K38</f>
-        <v>0.82114829008418799</v>
+        <v>0.82114829008418755</v>
       </c>
       <c r="L52" s="3">
         <f>J45*L36+K45*L37+L45*L38</f>
-        <v>0.57071489002111575</v>
+        <v>0.57071489002111631</v>
       </c>
       <c r="P52" s="3">
         <f>P45*P36+Q45*P37+R45*P38</f>
@@ -5798,11 +5808,11 @@
       </c>
       <c r="Q52" s="3">
         <f>P45*Q36+Q45*Q37+R45*Q38</f>
-        <v>0.82114729981928336</v>
+        <v>0.82114729981927925</v>
       </c>
       <c r="R52" s="3">
         <f>P45*R36+Q45*R37+R45*R38</f>
-        <v>0.57071631481805374</v>
+        <v>0.57071631481805973</v>
       </c>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.25">
@@ -5811,11 +5821,11 @@
       </c>
       <c r="B53">
         <f>SQRT(B48*B48+B49*B49+B50*B50)</f>
-        <v>26585702.041017018</v>
+        <v>26585702.052761097</v>
       </c>
       <c r="E53">
         <f t="shared" ref="E53:G53" si="1">SQRT(E48*E48+E49*E49+E50*E50)</f>
-        <v>26585702.384047892</v>
+        <v>26585702.374913916</v>
       </c>
       <c r="G53">
         <f t="shared" si="1"/>
@@ -5827,12 +5837,12 @@
         <v>111</v>
       </c>
       <c r="B54" s="18">
-        <f>B53-$G$53</f>
-        <v>-2.2511483877897263</v>
+        <f>$G$53-B53</f>
+        <v>2.239404309540987</v>
       </c>
       <c r="E54" s="29">
-        <f t="shared" ref="E54" si="2">E53-$G$53</f>
-        <v>-1.908117514103651</v>
+        <f>$G$53-E53</f>
+        <v>1.9172514900565147</v>
       </c>
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.25">
@@ -5846,13 +5856,13 @@
         <v>112</v>
       </c>
       <c r="B57" s="28">
-        <f>B48-G$48</f>
-        <v>0.97581280616577715</v>
+        <f>G$48-B48</f>
+        <v>-2.3197699257871136</v>
       </c>
       <c r="D57" s="28"/>
       <c r="E57" s="28">
-        <f>E48-G$48</f>
-        <v>-5.1352308817440644</v>
+        <f>G$48-E48</f>
+        <v>6.180533479549922</v>
       </c>
       <c r="G57" s="28"/>
     </row>
@@ -5861,12 +5871,12 @@
         <v>113</v>
       </c>
       <c r="B58" s="28">
-        <f>B49-G$49</f>
-        <v>-4.9376945309340954</v>
+        <f>G$49-B49</f>
+        <v>5.4487583041191101</v>
       </c>
       <c r="E58" s="28">
-        <f>E49-G$49</f>
-        <v>-2.1239041872322559</v>
+        <f>G$49-E49</f>
+        <v>1.7264111079275608</v>
       </c>
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.25">
@@ -5874,12 +5884,12 @@
         <v>114</v>
       </c>
       <c r="B59" s="28">
-        <f>B50-G$50</f>
-        <v>9.3208181280642748</v>
+        <f>G$50-B50</f>
+        <v>-11.101426205597818</v>
       </c>
       <c r="E59" s="28">
-        <f>E50-G$50</f>
-        <v>0.94050387013703585</v>
+        <f>G$50-E50</f>
+        <v>0.44441187474876642</v>
       </c>
     </row>
   </sheetData>
@@ -5892,13 +5902,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61604D80-09E5-4947-9F01-8E98FAA4B924}">
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.5703125" customWidth="1"/>
     <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5908,11 +5918,11 @@
       </c>
       <c r="B1">
         <f>Calculos!B18</f>
-        <v>-1.7532942457867327</v>
+        <v>-1.7532943320404997</v>
       </c>
       <c r="C1">
         <f>Calculos!E18</f>
-        <v>-1.7533351066769214</v>
+        <v>-1.7533350395906879</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -5945,11 +5955,11 @@
       </c>
       <c r="B5" s="30">
         <f>B$1+B$2*SIN(B4)-B4</f>
-        <v>-1.7532942457867327</v>
+        <v>-1.7532943320404997</v>
       </c>
       <c r="C5" s="30">
         <f>C$1+C$2*SIN(C4)-C4</f>
-        <v>-1.7533351066769214</v>
+        <v>-1.7533350395906879</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -5971,11 +5981,11 @@
       </c>
       <c r="B8">
         <f>B5/B6</f>
-        <v>1.7625114454919575</v>
+        <v>1.7625115321991669</v>
       </c>
       <c r="C8">
         <f>C5/C6</f>
-        <v>1.7625503547733024</v>
+        <v>1.7625502873344745</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.35">
@@ -5984,11 +5994,11 @@
       </c>
       <c r="B9">
         <f>B4-B8</f>
-        <v>-1.7625114454919575</v>
+        <v>-1.7625115321991669</v>
       </c>
       <c r="C9">
         <f>C4-C8</f>
-        <v>-1.7625503547733024</v>
+        <v>-1.7625502873344745</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -5997,11 +6007,11 @@
       </c>
       <c r="B10" s="30">
         <f>B$1+B$2*SIN(B9)-B9</f>
-        <v>4.0834286508064643E-3</v>
+        <v>4.0834291906490794E-3</v>
       </c>
       <c r="C10" s="30">
         <f>C$1+C$2*SIN(C9)-C9</f>
-        <v>4.0827161170104986E-3</v>
+        <v>4.0827156972182976E-3</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -6010,11 +6020,11 @@
       </c>
       <c r="B11" s="30">
         <f>B$2*COS(B9)-1</f>
-        <v>-1.0009964597344982</v>
+        <v>-1.0009964601796333</v>
       </c>
       <c r="C11" s="30">
         <f>C$2*COS(C9)-1</f>
-        <v>-1.0009964264596876</v>
+        <v>-1.0009964261135555</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -6023,24 +6033,24 @@
       </c>
       <c r="B13">
         <f>B10/B11</f>
-        <v>-4.0793637291080351E-3</v>
+        <v>-4.0793642665991944E-3</v>
       </c>
       <c r="C13">
         <f>C10/C11</f>
-        <v>-4.0786520401977873E-3</v>
+        <v>-4.0786516222338079E-3</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>74</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="45">
         <f>B9-B13</f>
-        <v>-1.7584320817628494</v>
+        <v>-1.7584321679325676</v>
       </c>
       <c r="C14">
         <f>C9-C13</f>
-        <v>-1.7584717027331045</v>
+        <v>-1.7584716357122407</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -6049,11 +6059,11 @@
       </c>
       <c r="B15" s="30">
         <f>B$1+B$2*SIN(B14)-B14</f>
-        <v>4.2727291926780708E-8</v>
+        <v>4.272730236287714E-8</v>
       </c>
       <c r="C15" s="30">
         <f>C$1+C$2*SIN(C14)-C14</f>
-        <v>4.2702076097356212E-8</v>
+        <v>4.2702068103750435E-8</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -6062,11 +6072,11 @@
       </c>
       <c r="B16" s="30">
         <f>B$2*COS(B14)-1</f>
-        <v>-1.0009755089820145</v>
+        <v>-1.0009755094247368</v>
       </c>
       <c r="C16">
         <f>C$2*COS(C14)-1</f>
-        <v>-1.0009754844177328</v>
+        <v>-1.0009754840734766</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -6075,24 +6085,24 @@
       </c>
       <c r="B18">
         <f>B15/B16</f>
-        <v>-4.2685651690153823E-8</v>
+        <v>-4.2685662097200188E-8</v>
       </c>
       <c r="C18">
         <f>C15/C16</f>
-        <v>-4.2660461481927301E-8</v>
+        <v>-4.2660453510783375E-8</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>75</v>
       </c>
-      <c r="B19" s="20">
+      <c r="B19" s="44">
         <f>B14-B18</f>
-        <v>-1.7584320390771977</v>
+        <v>-1.7584321252469055</v>
       </c>
       <c r="C19" s="20">
         <f>C14-C18</f>
-        <v>-1.7584716600726431</v>
+        <v>-1.7584715930517871</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -6114,11 +6124,11 @@
       </c>
       <c r="B21">
         <f>B$2*COS(B19)-1</f>
-        <v>-1.0009755087627046</v>
+        <v>-1.0009755092054267</v>
       </c>
       <c r="C21">
         <f>C$2*COS(C19)-1</f>
-        <v>-1.0009754841986052</v>
+        <v>-1.0009754838543488</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -6138,13 +6148,13 @@
       <c r="A24" t="s">
         <v>76</v>
       </c>
-      <c r="B24" s="20">
+      <c r="B24" s="44">
         <f>B19-B23</f>
-        <v>-1.7584320390771977</v>
+        <v>-1.7584321252469055</v>
       </c>
       <c r="C24" s="20">
         <f>C19-C23</f>
-        <v>-1.7584716600726431</v>
+        <v>-1.7584715930517871</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -6166,11 +6176,11 @@
       </c>
       <c r="B26">
         <f>B$2*COS(B24)-1</f>
-        <v>-1.0009755087627046</v>
+        <v>-1.0009755092054267</v>
       </c>
       <c r="C26">
         <f>C$2*COS(C24)-1</f>
-        <v>-1.0009754841986052</v>
+        <v>-1.0009754838543488</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>